<commit_message>
Expected Results fetched from Excel Sheet
</commit_message>
<xml_diff>
--- a/src/main/java/com/MercuryTours/qa/TestData/Test Data.xlsx
+++ b/src/main/java/com/MercuryTours/qa/TestData/Test Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\101139\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45269CA-4CAE-4F84-BB6B-3CC1B0318BEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95EF376-4FFD-428F-9040-3E3EE5180211}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Harsha</t>
   </si>
@@ -50,6 +51,42 @@
   </si>
   <si>
     <t>Harsha Subramanyam</t>
+  </si>
+  <si>
+    <t>TestCaseName</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Welcome: Mercury Tours</t>
+  </si>
+  <si>
+    <t>PageTitle_Home</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>REGISTER</t>
+  </si>
+  <si>
+    <t>PageTitle_Registration</t>
+  </si>
+  <si>
+    <t>Register: Mercury Tours</t>
+  </si>
+  <si>
+    <t>PageTitle_CarRentals</t>
+  </si>
+  <si>
+    <t>Under Construction: Mercury Tours</t>
+  </si>
+  <si>
+    <t>CarRentals</t>
+  </si>
+  <si>
+    <t>© 2005, Mercury Interactive (v. 011003-1.01-058)</t>
   </si>
 </sst>
 </file>
@@ -100,9 +137,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A24C76-04BA-4059-99A0-38E41E7F3591}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,4 +497,79 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA07CA22-7EA3-4B22-9B67-310925B1EB7A}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>